<commit_message>
Textgrids Type Pts 4-6, Speak textgrid pt 4, praat file pt 4
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEF3A78-D427-47D8-B0C2-62AA94202A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7600029D-02E8-4DB3-8463-27F62195A5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t>Participant</t>
   </si>
@@ -193,6 +193,18 @@
   </si>
   <si>
     <t>I got confused and did first the caja and then the language tasks.</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>Enara Ayala Pérez</t>
+  </si>
+  <si>
+    <t>I didn't tell them about the ñ and they used /n/ instead in muñeca and baño.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -283,38 +295,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -383,68 +400,6 @@
         <bottom/>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -759,23 +714,79 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
           <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="medium">
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
           <color rgb="FF000000"/>
-        </top>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -791,7 +802,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D7725C54-BC3C-4F16-BE30-EAEFD1E6A889}" name="Table2" displayName="Table2" ref="A1:L3" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowBorderDxfId="14" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D7725C54-BC3C-4F16-BE30-EAEFD1E6A889}" name="Table2" displayName="Table2" ref="A1:L3" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
   <autoFilter ref="A1:L3" xr:uid="{D7725C54-BC3C-4F16-BE30-EAEFD1E6A889}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{7424B4AF-20BB-4956-A693-DA5C2E491F93}" name="Nº" dataDxfId="13"/>
@@ -804,8 +815,8 @@
     <tableColumn id="8" xr3:uid="{2F9D02AD-A101-4502-9045-CD9C9E13C48F}" name="CAB" dataDxfId="6"/>
     <tableColumn id="9" xr3:uid="{85FF814B-2A7B-432F-8DAE-5AB34249AEB5}" name="RA" dataDxfId="5"/>
     <tableColumn id="10" xr3:uid="{0FC227E0-1B27-4152-863B-2CB8F32204E6}" name="INCIDENCES" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{503F2B95-E846-4929-AB22-0B04260E6C24}" name="Type_speed" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{EDCB596B-12D3-4EB1-8CF7-AAF9A3093A4F}" name="Type_accuracy" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{503F2B95-E846-4929-AB22-0B04260E6C24}" name="Type_speed" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{EDCB596B-12D3-4EB1-8CF7-AAF9A3093A4F}" name="Type_accuracy" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -818,10 +829,10 @@
     <tableColumn id="1" xr3:uid="{6A81B45A-EDC9-4FF5-8258-8648C067C16F}" name="Participant"/>
     <tableColumn id="5" xr3:uid="{23D0A20D-D062-4D9A-A44D-D77B8E1CBB39}" name="Name"/>
     <tableColumn id="10" xr3:uid="{706E71AC-2B72-418D-A17F-64B513C711DC}" name="ID"/>
-    <tableColumn id="4" xr3:uid="{7D21F159-CC51-40B5-A3A9-2FC35A1E3DC7}" name="Code" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{7D21F159-CC51-40B5-A3A9-2FC35A1E3DC7}" name="Code" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{0F7B8E20-170E-4530-BD6F-052C78EE98C3}" name="Version "/>
     <tableColumn id="3" xr3:uid="{C9573F81-3819-423D-82CC-5ABB8EA301BD}" name="List"/>
-    <tableColumn id="6" xr3:uid="{27B86DF5-6EF1-41B1-A9EC-9F0F5F275ADB}" name="Language_test" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{27B86DF5-6EF1-41B1-A9EC-9F0F5F275ADB}" name="Language_test" dataDxfId="0"/>
     <tableColumn id="9" xr3:uid="{89FF1955-3050-4A09-8388-44DB3C7BAF8D}" name="Date"/>
     <tableColumn id="13" xr3:uid="{0353A7A6-5360-4B04-A7A6-65360A0DB44E}" name="Notes"/>
     <tableColumn id="12" xr3:uid="{7D4D4D5D-E25F-4CB3-8EE9-5A89F5D57012}" name="SpanishAoA"/>
@@ -1271,7 +1282,7 @@
   <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1353,9 +1364,9 @@
       <c r="H2" s="4">
         <v>45240</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -1382,9 +1393,9 @@
       <c r="H3" s="4">
         <v>45240</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
@@ -1411,9 +1422,9 @@
       <c r="H4" s="4">
         <v>45240</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -1440,9 +1451,9 @@
       <c r="H5" s="4">
         <v>45246</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -1469,11 +1480,11 @@
       <c r="H6" s="4">
         <v>45246</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -1500,26 +1511,40 @@
       <c r="H7" s="4">
         <v>45246</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="2">
+        <v>11082</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
         <v>4</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="14">
+        <v>45250</v>
+      </c>
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -1595,6 +1620,9 @@
         <v>2</v>
       </c>
       <c r="G13" s="1"/>
+      <c r="I13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">

</xml_diff>

<commit_message>
Textgrids Speak pt 6, analysis files pts 1-6
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7600029D-02E8-4DB3-8463-27F62195A5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF020BD-8D6C-4A86-BE8F-0BB652968ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-156" yWindow="720" windowWidth="12516" windowHeight="12276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pilots" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>Participant</t>
   </si>
@@ -54,9 +54,6 @@
     <t>010101</t>
   </si>
   <si>
-    <t>20201</t>
-  </si>
-  <si>
     <t>030102</t>
   </si>
   <si>
@@ -205,6 +202,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Lucia Gomez Lopez</t>
+  </si>
+  <si>
+    <t>020201</t>
   </si>
 </sst>
 </file>
@@ -1157,54 +1160,54 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="K1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="C2" s="7">
         <v>9028</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="8">
         <v>45197</v>
@@ -1219,10 +1222,10 @@
         <v>3</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="K2">
         <v>28.48</v>
@@ -1233,16 +1236,16 @@
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="C3" s="10">
         <v>11527</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="12">
         <v>45087</v>
@@ -1257,10 +1260,10 @@
         <v>3</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K3">
         <v>28.48</v>
@@ -1282,7 +1285,7 @@
   <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1303,10 +1306,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1318,25 +1321,25 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>25</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1344,7 +1347,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3">
         <v>9383</v>
@@ -1359,7 +1362,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="4">
         <v>45240</v>
@@ -1373,13 +1376,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3">
         <v>11777</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1388,7 +1391,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="4">
         <v>45240</v>
@@ -1402,13 +1405,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3">
         <v>8424</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
@@ -1417,7 +1420,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="4">
         <v>45240</v>
@@ -1431,13 +1434,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3">
         <v>11787</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
@@ -1446,7 +1449,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="4">
         <v>45246</v>
@@ -1460,13 +1463,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3">
         <v>8542</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
@@ -1475,13 +1478,13 @@
         <v>3</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" s="4">
         <v>45246</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
@@ -1491,13 +1494,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
         <v>11587</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
@@ -1506,13 +1509,13 @@
         <v>3</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H7" s="4">
         <v>45246</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
@@ -1522,13 +1525,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="2">
         <v>11082</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
@@ -1537,36 +1540,50 @@
         <v>4</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H8" s="14">
         <v>45250</v>
       </c>
       <c r="I8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
+      <c r="B9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="2">
+        <v>11000</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2">
         <v>4</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="14">
+        <v>45251</v>
+      </c>
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1574,7 +1591,9 @@
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -1589,7 +1608,9 @@
       <c r="F11">
         <v>1</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1604,7 +1625,9 @@
       <c r="F12">
         <v>2</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -1619,9 +1642,11 @@
       <c r="F13">
         <v>2</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="I13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1637,7 +1662,9 @@
       <c r="F14">
         <v>3</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1652,7 +1679,9 @@
       <c r="F15">
         <v>3</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1667,7 +1696,9 @@
       <c r="F16">
         <v>4</v>
       </c>
-      <c r="G16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -1682,7 +1713,9 @@
       <c r="F17">
         <v>4</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -1697,7 +1730,9 @@
       <c r="F18">
         <v>1</v>
       </c>
-      <c r="G18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -1712,7 +1747,9 @@
       <c r="F19">
         <v>1</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -1727,7 +1764,9 @@
       <c r="F20">
         <v>2</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -1742,7 +1781,9 @@
       <c r="F21">
         <v>2</v>
       </c>
-      <c r="G21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -1757,7 +1798,9 @@
       <c r="F22">
         <v>3</v>
       </c>
-      <c r="G22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -1772,7 +1815,9 @@
       <c r="F23">
         <v>3</v>
       </c>
-      <c r="G23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -1787,7 +1832,9 @@
       <c r="F24">
         <v>4</v>
       </c>
-      <c r="G24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -1802,7 +1849,9 @@
       <c r="F25">
         <v>4</v>
       </c>
-      <c r="G25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -1817,7 +1866,9 @@
       <c r="F26">
         <v>1</v>
       </c>
-      <c r="G26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
@@ -1832,7 +1883,9 @@
       <c r="F27">
         <v>1</v>
       </c>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
@@ -1847,7 +1900,9 @@
       <c r="F28">
         <v>2</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
@@ -1862,7 +1917,9 @@
       <c r="F29">
         <v>2</v>
       </c>
-      <c r="G29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
@@ -1877,7 +1934,9 @@
       <c r="F30">
         <v>3</v>
       </c>
-      <c r="G30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
@@ -1892,7 +1951,9 @@
       <c r="F31">
         <v>3</v>
       </c>
-      <c r="G31" s="1"/>
+      <c r="G31" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
@@ -1907,7 +1968,9 @@
       <c r="F32">
         <v>4</v>
       </c>
-      <c r="G32" s="1"/>
+      <c r="G32" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
@@ -1922,7 +1985,9 @@
       <c r="F33">
         <v>4</v>
       </c>
-      <c r="G33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
@@ -1937,7 +2002,9 @@
       <c r="F34">
         <v>1</v>
       </c>
-      <c r="G34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
@@ -1952,7 +2019,9 @@
       <c r="F35">
         <v>1</v>
       </c>
-      <c r="G35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
@@ -1967,7 +2036,9 @@
       <c r="F36">
         <v>2</v>
       </c>
-      <c r="G36" s="1"/>
+      <c r="G36" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
@@ -1982,7 +2053,9 @@
       <c r="F37">
         <v>2</v>
       </c>
-      <c r="G37" s="1"/>
+      <c r="G37" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
@@ -1997,7 +2070,9 @@
       <c r="F38">
         <v>3</v>
       </c>
-      <c r="G38" s="1"/>
+      <c r="G38" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
@@ -2012,7 +2087,9 @@
       <c r="F39">
         <v>3</v>
       </c>
-      <c r="G39" s="1"/>
+      <c r="G39" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
@@ -2027,7 +2104,9 @@
       <c r="F40">
         <v>4</v>
       </c>
-      <c r="G40" s="1"/>
+      <c r="G40" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
@@ -2042,7 +2121,9 @@
       <c r="F41">
         <v>4</v>
       </c>
-      <c r="G41" s="1"/>
+      <c r="G41" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
@@ -2057,7 +2138,9 @@
       <c r="F42">
         <v>1</v>
       </c>
-      <c r="G42" s="1"/>
+      <c r="G42" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
@@ -2072,7 +2155,9 @@
       <c r="F43">
         <v>1</v>
       </c>
-      <c r="G43" s="1"/>
+      <c r="G43" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
@@ -2087,7 +2172,9 @@
       <c r="F44">
         <v>2</v>
       </c>
-      <c r="G44" s="1"/>
+      <c r="G44" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
@@ -2102,7 +2189,9 @@
       <c r="F45">
         <v>2</v>
       </c>
-      <c r="G45" s="1"/>
+      <c r="G45" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
@@ -2117,7 +2206,9 @@
       <c r="F46">
         <v>3</v>
       </c>
-      <c r="G46" s="1"/>
+      <c r="G46" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
@@ -2132,7 +2223,9 @@
       <c r="F47">
         <v>3</v>
       </c>
-      <c r="G47" s="1"/>
+      <c r="G47" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
@@ -2147,7 +2240,9 @@
       <c r="F48">
         <v>4</v>
       </c>
-      <c r="G48" s="1"/>
+      <c r="G48" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
@@ -2162,12 +2257,14 @@
       <c r="F49">
         <v>4</v>
       </c>
-      <c r="G49" s="1"/>
+      <c r="G49" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D2:D4 D5:D10" numberStoredAsText="1"/>
+    <ignoredError sqref="D2 D5:D10 D4" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Textgrids Speak and Type pts 7-8, analysis files
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF020BD-8D6C-4A86-BE8F-0BB652968ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DE9B56-53B9-4899-A323-3CBFC8EA4294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-156" yWindow="720" windowWidth="12516" windowHeight="12276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pilots" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
   <si>
     <t>Participant</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>020201</t>
+  </si>
+  <si>
+    <t>Diego Zabala Juarez</t>
+  </si>
+  <si>
+    <t>Typed-said the colour instead of the word in the first couple of trials in Practice 1. I corrected him and he did the rest correctly.</t>
   </si>
 </sst>
 </file>
@@ -298,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -324,6 +330,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1282,10 +1289,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:R49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1301,7 +1308,7 @@
     <col min="24" max="24" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1342,7 +1349,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1371,7 +1378,7 @@
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1400,7 +1407,7 @@
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1429,7 +1436,7 @@
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1458,7 +1465,7 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1489,7 +1496,7 @@
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1520,7 +1527,7 @@
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1549,7 +1556,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1578,10 +1585,16 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10">
+        <v>11893</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1594,8 +1607,14 @@
       <c r="G10" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H10" s="15">
+        <v>45252</v>
+      </c>
+      <c r="I10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1612,7 +1631,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1629,7 +1648,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1649,7 +1668,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1666,7 +1685,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1682,8 +1701,11 @@
       <c r="G15" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="R15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1700,7 +1722,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1717,7 +1739,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1734,7 +1756,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1751,7 +1773,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1768,7 +1790,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1785,7 +1807,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1802,7 +1824,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1819,7 +1841,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1836,7 +1858,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1852,8 +1874,11 @@
       <c r="G25" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1870,7 +1895,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1887,7 +1912,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1904,7 +1929,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1921,7 +1946,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1938,7 +1963,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1955,7 +1980,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Textgrid Type pt 9
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DE9B56-53B9-4899-A323-3CBFC8EA4294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34819538-EC19-4256-BF73-0B455F3E65CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
   <si>
     <t>Participant</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Typed-said the colour instead of the word in the first couple of trials in Practice 1. I corrected him and he did the rest correctly.</t>
+  </si>
+  <si>
+    <t>Catalina Platas Muñoz</t>
   </si>
 </sst>
 </file>
@@ -304,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -330,7 +333,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1291,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1586,28 +1588,28 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>11893</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="14">
         <v>45252</v>
       </c>
       <c r="I10" t="s">
@@ -1615,20 +1617,29 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="D11" s="1">
+      <c r="B11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="2">
+        <v>10439</v>
+      </c>
+      <c r="D11" s="13">
         <v>100201</v>
       </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>49</v>
+      </c>
+      <c r="H11" s="14">
+        <v>45253</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Textgrids Speak pt 9, Praat file
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34819538-EC19-4256-BF73-0B455F3E65CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFCF97A-6DE7-476D-8FAF-E164B8F34776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="684" windowWidth="12516" windowHeight="12276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pilots" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
   <si>
     <t>Participant</t>
   </si>
@@ -213,10 +213,25 @@
     <t>Diego Zabala Juarez</t>
   </si>
   <si>
-    <t>Typed-said the colour instead of the word in the first couple of trials in Practice 1. I corrected him and he did the rest correctly.</t>
-  </si>
-  <si>
     <t>Catalina Platas Muñoz</t>
+  </si>
+  <si>
+    <t>Irene Pereira López</t>
+  </si>
+  <si>
+    <t>Ana Fernández Rubio</t>
+  </si>
+  <si>
+    <t>Nerea Pérez Arriazu</t>
+  </si>
+  <si>
+    <t>Speaks fast. Tends to ¨cut¨ syllables in the sense that they are not heard clearly at all times. Typed-said the colour instead of the word in the first couple of trials in Practice 1. I corrected him and he did the rest correctly.</t>
+  </si>
+  <si>
+    <t>Haizea Lavega Torrado</t>
+  </si>
+  <si>
+    <t>Clara Lorenzo Tabueña</t>
   </si>
 </sst>
 </file>
@@ -307,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -333,6 +348,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1293,8 +1309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1613,7 +1629,7 @@
         <v>45252</v>
       </c>
       <c r="I10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -1621,7 +1637,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2">
         <v>10439</v>
@@ -1643,63 +1659,96 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="D12" s="1">
+      <c r="B12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="2">
+        <v>11570</v>
+      </c>
+      <c r="D12" s="13">
         <v>110102</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>51</v>
       </c>
+      <c r="H12" s="14">
+        <v>45257</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="D13" s="1">
+      <c r="B13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="2">
+        <v>9754</v>
+      </c>
+      <c r="D13" s="13">
         <v>120202</v>
       </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="13" t="s">
         <v>22</v>
+      </c>
+      <c r="H13" s="14">
+        <v>45257</v>
       </c>
       <c r="I13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="D14" s="1">
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="2">
+        <v>10344</v>
+      </c>
+      <c r="D14" s="13">
         <v>130103</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
         <v>3</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="13" t="s">
         <v>44</v>
+      </c>
+      <c r="H14" s="14">
+        <v>45257</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15">
+        <v>11614</v>
+      </c>
       <c r="D15" s="1">
         <v>140203</v>
       </c>
@@ -1711,6 +1760,9 @@
       </c>
       <c r="G15" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="H15" s="15">
+        <v>45258</v>
       </c>
       <c r="R15" t="s">
         <v>54</v>
@@ -1720,6 +1772,12 @@
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16">
+        <v>11782</v>
+      </c>
       <c r="D16" s="1">
         <v>150104</v>
       </c>
@@ -1731,6 +1789,9 @@
       </c>
       <c r="G16" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="H16" s="15">
+        <v>45258</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Textgrids Speak, Praat files pt 12
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E783430F-9326-4D1D-8C44-5B3098229593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA45137A-51C3-4C17-B47A-0939103401E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="89">
   <si>
     <t>Participant</t>
   </si>
@@ -241,13 +241,76 @@
   </si>
   <si>
     <t>Spoke in many type trials. Has some very late Speak trials (responds after 1200ms). Was not very concentrated -- many mistakes in the colour-cue. Very long durations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sofía Puerta Cabiró </t>
+  </si>
+  <si>
+    <t>Tania Vidar Cascallar</t>
+  </si>
+  <si>
+    <t>Marta Buendía Méndez</t>
+  </si>
+  <si>
+    <t>Lucía Rodríguez Ezquerro</t>
+  </si>
+  <si>
+    <t>Visual lexical decision task (C02) did not work to the end. After a few words the fixation cross appeared and then did not proceed to another word or task. We attempted it a second time, nothing. We completed the rest of the langauge tasks (without run non-stop) and I was in the room.</t>
+  </si>
+  <si>
+    <t>Practice 1: She thought she had to name the colour. I corrected her and she got trials 5-12  right.</t>
+  </si>
+  <si>
+    <t>Familiarisation: many hesitations, but did not repeat during Practices. She restarted the language tasks after having completed them. There are two output files for the written task.</t>
+  </si>
+  <si>
+    <t>Gorka Zubizarreta Calvo</t>
+  </si>
+  <si>
+    <t>Marta Pérez Verdugo</t>
+  </si>
+  <si>
+    <t>Maria Garcia Revilla</t>
+  </si>
+  <si>
+    <t>Mei Muñoz Ruiz</t>
+  </si>
+  <si>
+    <t>Check his RTs. Seemed a bit slow during the Practice sessions.</t>
+  </si>
+  <si>
+    <t>Beatriz Saiz Saiz</t>
+  </si>
+  <si>
+    <t>Nerea Segura Saez</t>
+  </si>
+  <si>
+    <t>Begoña Urrutia González</t>
+  </si>
+  <si>
+    <t>Ana Trespalacios Rivera</t>
+  </si>
+  <si>
+    <t>FechaNacimiento</t>
+  </si>
+  <si>
+    <t>Sexo</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,6 +322,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="161"/>
@@ -279,7 +349,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -327,11 +397,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -357,11 +436,33 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="19">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -838,39 +939,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D7725C54-BC3C-4F16-BE30-EAEFD1E6A889}" name="Table2" displayName="Table2" ref="A1:L3" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
-  <autoFilter ref="A1:L3" xr:uid="{D7725C54-BC3C-4F16-BE30-EAEFD1E6A889}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{7424B4AF-20BB-4956-A693-DA5C2E491F93}" name="Nº" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{D26CEDE0-6675-4478-AE1C-23ABA5C453CA}" name="NOMBRE" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{EFE7765A-783D-40C2-88ED-FBD03D4624CF}" name="ID" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{44B7B9A7-3620-4B2C-AA1F-A445ABB5A4AB}" name="CODE" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{53BF4CCF-E2C8-4075-828B-045D44DC2B5B}" name="DATE" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{1B290470-E23F-485F-AC08-FFFEAC9F056D}" name="VERSION" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{F0145F60-BB11-4B87-9FCD-BDAB0F3EDDB5}" name="LIST" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{2F9D02AD-A101-4502-9045-CD9C9E13C48F}" name="CAB" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{85FF814B-2A7B-432F-8DAE-5AB34249AEB5}" name="RA" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{0FC227E0-1B27-4152-863B-2CB8F32204E6}" name="INCIDENCES" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{503F2B95-E846-4929-AB22-0B04260E6C24}" name="Type_speed" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{EDCB596B-12D3-4EB1-8CF7-AAF9A3093A4F}" name="Type_accuracy" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D7725C54-BC3C-4F16-BE30-EAEFD1E6A889}" name="Table2" displayName="Table2" ref="A1:N3" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15">
+  <autoFilter ref="A1:N3" xr:uid="{D7725C54-BC3C-4F16-BE30-EAEFD1E6A889}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{7424B4AF-20BB-4956-A693-DA5C2E491F93}" name="Nº" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{D26CEDE0-6675-4478-AE1C-23ABA5C453CA}" name="NOMBRE" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{EFE7765A-783D-40C2-88ED-FBD03D4624CF}" name="ID" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{44B7B9A7-3620-4B2C-AA1F-A445ABB5A4AB}" name="CODE" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{53BF4CCF-E2C8-4075-828B-045D44DC2B5B}" name="DATE" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{1015A516-CB69-4FC3-87A7-C4A13E267A67}" name="FechaNacimiento"/>
+    <tableColumn id="14" xr3:uid="{EA8F05D9-3EE2-477E-9DA0-F765608E29F0}" name="Sexo"/>
+    <tableColumn id="6" xr3:uid="{1B290470-E23F-485F-AC08-FFFEAC9F056D}" name="VERSION" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{F0145F60-BB11-4B87-9FCD-BDAB0F3EDDB5}" name="LIST" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{2F9D02AD-A101-4502-9045-CD9C9E13C48F}" name="CAB" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{85FF814B-2A7B-432F-8DAE-5AB34249AEB5}" name="RA" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{0FC227E0-1B27-4152-863B-2CB8F32204E6}" name="INCIDENCES" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{503F2B95-E846-4929-AB22-0B04260E6C24}" name="Type_speed" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{EDCB596B-12D3-4EB1-8CF7-AAF9A3093A4F}" name="Type_accuracy" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}" name="Table1" displayName="Table1" ref="A1:M49" totalsRowShown="0">
-  <autoFilter ref="A1:M49" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}" name="Table1" displayName="Table1" ref="A1:O49" totalsRowShown="0">
+  <autoFilter ref="A1:O49" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{6A81B45A-EDC9-4FF5-8258-8648C067C16F}" name="Participant"/>
     <tableColumn id="5" xr3:uid="{23D0A20D-D062-4D9A-A44D-D77B8E1CBB39}" name="Name"/>
     <tableColumn id="10" xr3:uid="{706E71AC-2B72-418D-A17F-64B513C711DC}" name="ID"/>
-    <tableColumn id="4" xr3:uid="{7D21F159-CC51-40B5-A3A9-2FC35A1E3DC7}" name="Code" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{7D21F159-CC51-40B5-A3A9-2FC35A1E3DC7}" name="Code" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{0F7B8E20-170E-4530-BD6F-052C78EE98C3}" name="Version "/>
     <tableColumn id="3" xr3:uid="{C9573F81-3819-423D-82CC-5ABB8EA301BD}" name="List"/>
-    <tableColumn id="6" xr3:uid="{27B86DF5-6EF1-41B1-A9EC-9F0F5F275ADB}" name="Language_test" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{27B86DF5-6EF1-41B1-A9EC-9F0F5F275ADB}" name="Language_test" dataDxfId="1"/>
     <tableColumn id="9" xr3:uid="{89FF1955-3050-4A09-8388-44DB3C7BAF8D}" name="Date"/>
     <tableColumn id="13" xr3:uid="{0353A7A6-5360-4B04-A7A6-65360A0DB44E}" name="Notes"/>
+    <tableColumn id="14" xr3:uid="{4580F522-AB7C-463E-B145-EBE3420458C5}" name="FechaNacimiento"/>
+    <tableColumn id="15" xr3:uid="{E351B0AB-595F-4765-9989-9C66FD2C2557}" name="Sexo" dataDxfId="0"/>
     <tableColumn id="12" xr3:uid="{7D4D4D5D-E25F-4CB3-8EE9-5A89F5D57012}" name="SpanishAoA"/>
     <tableColumn id="11" xr3:uid="{F2E1F23C-70DF-440E-B763-D813108EF947}" name="BEST"/>
     <tableColumn id="8" xr3:uid="{4C118AC6-F397-4959-8D77-72283767A378}" name="Type_speed"/>
@@ -1177,21 +1282,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5136CCB-2A52-4B66-B376-BBDF6C18D45E}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.5546875" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" customWidth="1"/>
+    <col min="6" max="7" width="10.5546875" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
@@ -1208,28 +1314,34 @@
         <v>29</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>35</v>
       </c>
@@ -1245,29 +1357,35 @@
       <c r="E2" s="8">
         <v>45197</v>
       </c>
-      <c r="F2" s="6">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6">
-        <v>1</v>
+      <c r="F2" s="8">
+        <v>36624</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6">
         <v>3</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>28.48</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>96.9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>39</v>
       </c>
@@ -1283,29 +1401,36 @@
       <c r="E3" s="12">
         <v>45087</v>
       </c>
-      <c r="F3" s="9">
-        <v>2</v>
-      </c>
-      <c r="G3" s="9">
-        <v>1</v>
+      <c r="F3" s="12">
+        <v>37810</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>88</v>
       </c>
       <c r="H3" s="9">
+        <v>2</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9">
         <v>3</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>28.48</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>96.9</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1315,26 +1440,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
-  <dimension ref="A1:R49"/>
+  <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="12" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" customWidth="1"/>
     <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.5546875" customWidth="1"/>
-    <col min="12" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" style="20" customWidth="1"/>
+    <col min="12" max="13" width="10.5546875" customWidth="1"/>
+    <col min="14" max="15" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1363,19 +1492,25 @@
         <v>46</v>
       </c>
       <c r="J1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1401,10 +1536,16 @@
         <v>45240</v>
       </c>
       <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J2" s="12">
+        <v>36910</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1430,10 +1571,16 @@
         <v>45240</v>
       </c>
       <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J3" s="12">
+        <v>36978</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1459,10 +1606,16 @@
         <v>45240</v>
       </c>
       <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J4" s="12">
+        <v>36484</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1488,10 +1641,16 @@
         <v>45246</v>
       </c>
       <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J5" s="12">
+        <v>36631</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1519,10 +1678,16 @@
       <c r="I6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J6" s="12">
+        <v>33073</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1550,10 +1715,16 @@
       <c r="I7" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J7" s="12">
+        <v>38338</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1581,8 +1752,14 @@
       <c r="I8" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J8" s="16">
+        <v>37166</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1610,8 +1787,14 @@
       <c r="I9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J9" s="16">
+        <v>37264</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1639,8 +1822,14 @@
       <c r="I10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J10" s="16">
+        <v>37200</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1668,8 +1857,14 @@
       <c r="I11" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J11" s="16">
+        <v>36893</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1694,8 +1889,14 @@
       <c r="H12" s="14">
         <v>45257</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J12" s="16">
+        <v>37880</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1723,8 +1924,14 @@
       <c r="I13" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J13" s="19">
+        <v>37460</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1749,8 +1956,14 @@
       <c r="H14" s="14">
         <v>45257</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J14" s="16">
+        <v>37504</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1775,11 +1988,17 @@
       <c r="H15" s="14">
         <v>45258</v>
       </c>
-      <c r="R15" t="s">
+      <c r="J15" s="16">
+        <v>38214</v>
+      </c>
+      <c r="K15" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="T15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1804,8 +2023,14 @@
       <c r="H16" s="14">
         <v>45258</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J16" s="16">
+        <v>37691</v>
+      </c>
+      <c r="K16" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1833,215 +2058,419 @@
       <c r="I17" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="J17" s="16">
+        <v>34028</v>
+      </c>
+      <c r="K17" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="D18" s="1">
+      <c r="B18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="2">
+        <v>11438</v>
+      </c>
+      <c r="D18" s="13">
         <v>170101</v>
       </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="s">
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="H18" s="14">
+        <v>45260</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J18" s="12">
+        <v>38244</v>
+      </c>
+      <c r="K18" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="D19" s="1">
+      <c r="B19" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="15">
+        <v>2293</v>
+      </c>
+      <c r="D19" s="13">
         <v>180201</v>
       </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="E19" s="2">
+        <v>2</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="H19" s="14">
+        <v>45260</v>
+      </c>
+      <c r="I19" t="s">
+        <v>73</v>
+      </c>
+      <c r="J19" s="16">
+        <v>32903</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="D20" s="1">
+      <c r="B20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="3">
+        <v>9818</v>
+      </c>
+      <c r="D20" s="13">
         <v>190102</v>
       </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1" t="s">
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2</v>
+      </c>
+      <c r="G20" s="13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="H20" s="14">
+        <v>45260</v>
+      </c>
+      <c r="I20" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" s="16">
+        <v>37433</v>
+      </c>
+      <c r="K20" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="D21" s="1">
+      <c r="B21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="3">
+        <v>10983</v>
+      </c>
+      <c r="D21" s="13">
         <v>200202</v>
       </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1" t="s">
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2</v>
+      </c>
+      <c r="G21" s="13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="H21" s="14">
+        <v>45260</v>
+      </c>
+      <c r="J21" s="16">
+        <v>37936</v>
+      </c>
+      <c r="K21" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="D22" s="1">
+      <c r="B22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="3">
+        <v>11478</v>
+      </c>
+      <c r="D22" s="13">
         <v>210103</v>
       </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
         <v>3</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="H22" s="14">
+        <v>45261</v>
+      </c>
+      <c r="I22" t="s">
+        <v>79</v>
+      </c>
+      <c r="J22" s="16">
+        <v>34393</v>
+      </c>
+      <c r="K22" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="D23" s="1">
+      <c r="B23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="2">
+        <v>10464</v>
+      </c>
+      <c r="D23" s="13">
         <v>220203</v>
       </c>
-      <c r="E23">
-        <v>2</v>
-      </c>
-      <c r="F23">
+      <c r="E23" s="2">
+        <v>2</v>
+      </c>
+      <c r="F23" s="2">
         <v>3</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="H23" s="14">
+        <v>45261</v>
+      </c>
+      <c r="J23" s="16">
+        <v>35659</v>
+      </c>
+      <c r="K23" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="D24" s="1">
+      <c r="B24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="2">
+        <v>10637</v>
+      </c>
+      <c r="D24" s="13">
         <v>230104</v>
       </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
         <v>4</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="H24" s="14">
+        <v>45261</v>
+      </c>
+      <c r="I24" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="16">
+        <v>37869</v>
+      </c>
+      <c r="K24" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="M24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="D25" s="1">
+      <c r="B25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="2">
+        <v>10443</v>
+      </c>
+      <c r="D25" s="13">
         <v>240204</v>
       </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-      <c r="F25">
+      <c r="E25" s="2">
+        <v>2</v>
+      </c>
+      <c r="F25" s="2">
         <v>4</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="R25" t="s">
+      <c r="H25" s="14">
+        <v>45261</v>
+      </c>
+      <c r="J25" s="16">
+        <v>37670</v>
+      </c>
+      <c r="K25" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="T25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="D26" s="1">
+      <c r="B26" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="15">
+        <v>11512</v>
+      </c>
+      <c r="D26" s="13">
         <v>250101</v>
       </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1" t="s">
+      <c r="E26" s="2">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="H26" s="14">
+        <v>45264</v>
+      </c>
+      <c r="J26" s="16">
+        <v>37838</v>
+      </c>
+      <c r="K26" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="D27" s="1">
+      <c r="B27" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="3">
+        <v>11124</v>
+      </c>
+      <c r="D27" s="13">
         <v>260201</v>
       </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+      <c r="G27" s="13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="H27" s="14">
+        <v>45264</v>
+      </c>
+      <c r="J27" s="16">
+        <v>37040</v>
+      </c>
+      <c r="K27" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="D28" s="1">
+      <c r="B28" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="3">
+        <v>11600</v>
+      </c>
+      <c r="D28" s="13">
         <v>270102</v>
       </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1" t="s">
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2">
+        <v>2</v>
+      </c>
+      <c r="G28" s="13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="H28" s="14">
+        <v>45264</v>
+      </c>
+      <c r="J28" s="16">
+        <v>38142</v>
+      </c>
+      <c r="K28" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="D29" s="1">
+      <c r="B29" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="3">
+        <v>3061</v>
+      </c>
+      <c r="D29" s="13">
         <v>280202</v>
       </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-      <c r="F29">
-        <v>2</v>
-      </c>
-      <c r="G29" s="1" t="s">
+      <c r="E29" s="2">
+        <v>2</v>
+      </c>
+      <c r="F29" s="2">
+        <v>2</v>
+      </c>
+      <c r="G29" s="13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H29" s="14">
+        <v>45264</v>
+      </c>
+      <c r="J29" s="16">
+        <v>33365</v>
+      </c>
+      <c r="K29" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2058,7 +2487,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2075,7 +2504,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Textgrid Speak pt 16, textgrid Type pt 18
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA45137A-51C3-4C17-B47A-0939103401E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C9669E-CB31-484E-BBC3-C7C35DE1EB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="104">
   <si>
     <t>Participant</t>
   </si>
@@ -304,6 +304,51 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Leire Rodriguez Roman</t>
+  </si>
+  <si>
+    <t>Amparo Gómez Cuevas</t>
+  </si>
+  <si>
+    <t>Isabel García De las Cuevas</t>
+  </si>
+  <si>
+    <t>Marina Vásquez Vicuña</t>
+  </si>
+  <si>
+    <t>Typing questionnaire: I pressed enter before entering my code for the participant, so there is only the ID from Participa.</t>
+  </si>
+  <si>
+    <t>Alvaro Alaba</t>
+  </si>
+  <si>
+    <t>Elena Ruiz Sandoya</t>
+  </si>
+  <si>
+    <t>Maider Ormaetxea Fernández</t>
+  </si>
+  <si>
+    <t>Diego Garcia-Mercadal Mendicuti</t>
+  </si>
+  <si>
+    <t>Eider Vazquez Garrido</t>
+  </si>
+  <si>
+    <t>Irene Lopez Muro</t>
+  </si>
+  <si>
+    <t>Elisa Sanchez Bayona</t>
+  </si>
+  <si>
+    <t>Inés Martínez Ortega</t>
+  </si>
+  <si>
+    <t>Super long nails</t>
+  </si>
+  <si>
+    <t>Eider De la Torre Moreno</t>
   </si>
 </sst>
 </file>
@@ -410,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -438,22 +483,19 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -986,9 +1028,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1026,7 +1068,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1132,7 +1174,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1274,7 +1316,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1442,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:H29"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1455,7 +1497,7 @@
     <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.44140625" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" style="20" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" style="19" customWidth="1"/>
     <col min="12" max="13" width="10.5546875" customWidth="1"/>
     <col min="14" max="15" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -1494,7 +1536,7 @@
       <c r="J1" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="20" t="s">
         <v>85</v>
       </c>
       <c r="L1" t="s">
@@ -1539,7 +1581,7 @@
       <c r="J2" s="12">
         <v>36910</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="9" t="s">
         <v>88</v>
       </c>
       <c r="L2" s="12"/>
@@ -1574,7 +1616,7 @@
       <c r="J3" s="12">
         <v>36978</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="9" t="s">
         <v>88</v>
       </c>
       <c r="L3" s="12"/>
@@ -1609,7 +1651,7 @@
       <c r="J4" s="12">
         <v>36484</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="9" t="s">
         <v>88</v>
       </c>
       <c r="L4" s="12"/>
@@ -1644,7 +1686,7 @@
       <c r="J5" s="12">
         <v>36631</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="9" t="s">
         <v>88</v>
       </c>
       <c r="L5" s="12"/>
@@ -1681,7 +1723,7 @@
       <c r="J6" s="12">
         <v>33073</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="9" t="s">
         <v>88</v>
       </c>
       <c r="L6" s="12"/>
@@ -1718,7 +1760,7 @@
       <c r="J7" s="12">
         <v>38338</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="9" t="s">
         <v>88</v>
       </c>
       <c r="L7" s="12"/>
@@ -1755,7 +1797,7 @@
       <c r="J8" s="16">
         <v>37166</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1790,7 +1832,7 @@
       <c r="J9" s="16">
         <v>37264</v>
       </c>
-      <c r="K9" s="21" t="s">
+      <c r="K9" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1825,7 +1867,7 @@
       <c r="J10" s="16">
         <v>37200</v>
       </c>
-      <c r="K10" s="20" t="s">
+      <c r="K10" s="19" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1860,7 +1902,7 @@
       <c r="J11" s="16">
         <v>36893</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="K11" s="19" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1892,7 +1934,7 @@
       <c r="J12" s="16">
         <v>37880</v>
       </c>
-      <c r="K12" s="20" t="s">
+      <c r="K12" s="19" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1924,10 +1966,10 @@
       <c r="I13" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="16">
         <v>37460</v>
       </c>
-      <c r="K13" s="20" t="s">
+      <c r="K13" s="19" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1959,7 +2001,7 @@
       <c r="J14" s="16">
         <v>37504</v>
       </c>
-      <c r="K14" s="20" t="s">
+      <c r="K14" s="19" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1991,7 +2033,7 @@
       <c r="J15" s="16">
         <v>38214</v>
       </c>
-      <c r="K15" s="20" t="s">
+      <c r="K15" s="19" t="s">
         <v>87</v>
       </c>
       <c r="T15" t="s">
@@ -2026,7 +2068,7 @@
       <c r="J16" s="16">
         <v>37691</v>
       </c>
-      <c r="K16" s="20" t="s">
+      <c r="K16" s="19" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2061,7 +2103,7 @@
       <c r="J17" s="16">
         <v>34028</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="K17" s="19" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2096,7 +2138,7 @@
       <c r="J18" s="12">
         <v>38244</v>
       </c>
-      <c r="K18" s="20" t="s">
+      <c r="K18" s="19" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2131,7 +2173,7 @@
       <c r="J19" s="16">
         <v>32903</v>
       </c>
-      <c r="K19" s="20" t="s">
+      <c r="K19" s="19" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2166,7 +2208,7 @@
       <c r="J20" s="16">
         <v>37433</v>
       </c>
-      <c r="K20" s="20" t="s">
+      <c r="K20" s="19" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2198,7 +2240,7 @@
       <c r="J21" s="16">
         <v>37936</v>
       </c>
-      <c r="K21" s="20" t="s">
+      <c r="K21" s="19" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2233,7 +2275,7 @@
       <c r="J22" s="16">
         <v>34393</v>
       </c>
-      <c r="K22" s="20" t="s">
+      <c r="K22" s="19" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2265,7 +2307,7 @@
       <c r="J23" s="16">
         <v>35659</v>
       </c>
-      <c r="K23" s="20" t="s">
+      <c r="K23" s="19" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2300,7 +2342,7 @@
       <c r="J24" s="16">
         <v>37869</v>
       </c>
-      <c r="K24" s="20" t="s">
+      <c r="K24" s="19" t="s">
         <v>88</v>
       </c>
       <c r="M24" t="s">
@@ -2335,7 +2377,7 @@
       <c r="J25" s="16">
         <v>37670</v>
       </c>
-      <c r="K25" s="20" t="s">
+      <c r="K25" s="19" t="s">
         <v>88</v>
       </c>
       <c r="T25" t="s">
@@ -2370,7 +2412,7 @@
       <c r="J26" s="16">
         <v>37838</v>
       </c>
-      <c r="K26" s="20" t="s">
+      <c r="K26" s="19" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2402,7 +2444,7 @@
       <c r="J27" s="16">
         <v>37040</v>
       </c>
-      <c r="K27" s="20" t="s">
+      <c r="K27" s="19" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2434,7 +2476,7 @@
       <c r="J28" s="16">
         <v>38142</v>
       </c>
-      <c r="K28" s="20" t="s">
+      <c r="K28" s="19" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2466,232 +2508,436 @@
       <c r="J29" s="16">
         <v>33365</v>
       </c>
-      <c r="K29" s="20" t="s">
+      <c r="K29" s="19" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="D30" s="1">
+      <c r="B30" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="3">
+        <v>11527</v>
+      </c>
+      <c r="D30" s="13">
         <v>290103</v>
       </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30">
+      <c r="E30" s="2">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2">
         <v>3</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="13" t="s">
         <v>43</v>
       </c>
+      <c r="H30" s="14">
+        <v>45265</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="J30" s="16">
+        <v>37810</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="D31" s="1">
+      <c r="B31" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2317</v>
+      </c>
+      <c r="D31" s="13">
         <v>300203</v>
       </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-      <c r="F31">
+      <c r="E31" s="2">
+        <v>2</v>
+      </c>
+      <c r="F31" s="2">
         <v>3</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="13" t="s">
         <v>48</v>
       </c>
+      <c r="H31" s="14">
+        <v>45265</v>
+      </c>
+      <c r="J31" s="16">
+        <v>33146</v>
+      </c>
+      <c r="K31" s="19" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="D32" s="1">
+      <c r="B32" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="3">
+        <v>8175</v>
+      </c>
+      <c r="D32" s="13">
         <v>310104</v>
       </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="F32">
+      <c r="E32" s="2">
+        <v>1</v>
+      </c>
+      <c r="F32" s="2">
         <v>4</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="H32" s="14">
+        <v>45265</v>
+      </c>
+      <c r="J32" s="16">
+        <v>32922</v>
+      </c>
+      <c r="K32" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="D33" s="1">
+      <c r="B33" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1697</v>
+      </c>
+      <c r="D33" s="13">
         <v>320204</v>
       </c>
-      <c r="E33">
-        <v>2</v>
-      </c>
-      <c r="F33">
+      <c r="E33" s="2">
+        <v>2</v>
+      </c>
+      <c r="F33" s="2">
         <v>4</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34">
+      <c r="H33" s="14">
+        <v>45265</v>
+      </c>
+      <c r="J33" s="16">
+        <v>32661</v>
+      </c>
+      <c r="K33" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="D34" s="1">
+      <c r="B34" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="2">
+        <v>9039</v>
+      </c>
+      <c r="D34" s="13">
         <v>330101</v>
       </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34" s="1" t="s">
+      <c r="E34" s="2">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="H34" s="21">
+        <v>45271</v>
+      </c>
+      <c r="J34" s="16">
+        <v>35705</v>
+      </c>
+      <c r="K34" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="D35" s="1">
+      <c r="B35" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="3">
+        <v>10010</v>
+      </c>
+      <c r="D35" s="13">
         <v>340201</v>
       </c>
-      <c r="E35">
-        <v>2</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35" s="1" t="s">
+      <c r="E35" s="2">
+        <v>2</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1</v>
+      </c>
+      <c r="G35" s="13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="H35" s="4">
+        <v>45272</v>
+      </c>
+      <c r="J35" s="16">
+        <v>37475</v>
+      </c>
+      <c r="K35" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="D36" s="1">
+      <c r="B36" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="3">
+        <v>10415</v>
+      </c>
+      <c r="D36" s="13">
         <v>350102</v>
       </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36">
-        <v>2</v>
-      </c>
-      <c r="G36" s="1" t="s">
+      <c r="E36" s="2">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2">
+        <v>2</v>
+      </c>
+      <c r="G36" s="13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="H36" s="4">
+        <v>45272</v>
+      </c>
+      <c r="J36" s="16">
+        <v>37515</v>
+      </c>
+      <c r="K36" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
         <v>36</v>
       </c>
-      <c r="D37" s="1">
+      <c r="B37" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="3">
+        <v>6729</v>
+      </c>
+      <c r="D37" s="13">
         <v>360202</v>
       </c>
-      <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="F37">
-        <v>2</v>
-      </c>
-      <c r="G37" s="1" t="s">
+      <c r="E37" s="2">
+        <v>2</v>
+      </c>
+      <c r="F37" s="2">
+        <v>2</v>
+      </c>
+      <c r="G37" s="13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="H37" s="4">
+        <v>45272</v>
+      </c>
+      <c r="J37" s="16">
+        <v>34059</v>
+      </c>
+      <c r="K37" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="D38" s="1">
+      <c r="B38" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="3">
+        <v>11066</v>
+      </c>
+      <c r="D38" s="13">
         <v>370103</v>
       </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
+      <c r="E38" s="2">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2">
         <v>3</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="H38" s="14">
+        <v>45273</v>
+      </c>
+      <c r="I38" t="s">
+        <v>66</v>
+      </c>
+      <c r="J38" s="16">
+        <v>37152</v>
+      </c>
+      <c r="K38" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="D39" s="1">
+      <c r="B39" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="2">
+        <v>9245</v>
+      </c>
+      <c r="D39" s="13">
         <v>380203</v>
       </c>
-      <c r="E39">
-        <v>2</v>
-      </c>
-      <c r="F39">
+      <c r="E39" s="2">
+        <v>2</v>
+      </c>
+      <c r="F39" s="2">
         <v>3</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="H39" s="14">
+        <v>45273</v>
+      </c>
+      <c r="I39" t="s">
+        <v>102</v>
+      </c>
+      <c r="J39" s="16">
+        <v>36607</v>
+      </c>
+      <c r="K39" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
         <v>39</v>
       </c>
-      <c r="D40" s="1">
+      <c r="B40" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="2">
+        <v>11067</v>
+      </c>
+      <c r="D40" s="13">
         <v>390104</v>
       </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40">
+      <c r="E40" s="2">
+        <v>1</v>
+      </c>
+      <c r="F40" s="2">
         <v>4</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G40" s="13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="H40" s="14">
+        <v>45273</v>
+      </c>
+      <c r="J40" s="16">
+        <v>35101</v>
+      </c>
+      <c r="K40" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
         <v>40</v>
       </c>
-      <c r="D41" s="1">
+      <c r="B41" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="2">
+        <v>8819</v>
+      </c>
+      <c r="D41" s="13">
         <v>400204</v>
       </c>
-      <c r="E41">
-        <v>2</v>
-      </c>
-      <c r="F41">
+      <c r="E41" s="2">
+        <v>2</v>
+      </c>
+      <c r="F41" s="2">
         <v>4</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G41" s="13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42">
+      <c r="H41" s="14">
+        <v>45273</v>
+      </c>
+      <c r="J41" s="16">
+        <v>35856</v>
+      </c>
+      <c r="K41" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
         <v>41</v>
       </c>
-      <c r="D42" s="1">
+      <c r="B42" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="15">
+        <v>6210</v>
+      </c>
+      <c r="D42" s="13">
         <v>410101</v>
       </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42" s="1" t="s">
+      <c r="E42" s="2">
+        <v>1</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1</v>
+      </c>
+      <c r="G42" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" s="14">
+        <v>45274</v>
+      </c>
+      <c r="J42" s="16">
+        <v>35934</v>
+      </c>
+      <c r="K42" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2708,7 +2954,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2724,8 +2970,11 @@
       <c r="G44" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K44" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2742,7 +2991,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2759,7 +3008,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2776,7 +3025,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Textgrid Speak pts 18-21, Praat files
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C9669E-CB31-484E-BBC3-C7C35DE1EB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79240AD-F31B-449D-B651-DF9815DBC82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -258,9 +258,6 @@
     <t>Visual lexical decision task (C02) did not work to the end. After a few words the fixation cross appeared and then did not proceed to another word or task. We attempted it a second time, nothing. We completed the rest of the langauge tasks (without run non-stop) and I was in the room.</t>
   </si>
   <si>
-    <t>Practice 1: She thought she had to name the colour. I corrected her and she got trials 5-12  right.</t>
-  </si>
-  <si>
     <t>Familiarisation: many hesitations, but did not repeat during Practices. She restarted the language tasks after having completed them. There are two output files for the written task.</t>
   </si>
   <si>
@@ -349,6 +346,9 @@
   </si>
   <si>
     <t>Eider De la Torre Moreno</t>
+  </si>
+  <si>
+    <t>Practice 1: She thought she had to name the colour. I corrected her and she got trials 5-12  right. Rather slow RTs. Speaks slowly.</t>
   </si>
 </sst>
 </file>
@@ -1356,10 +1356,10 @@
         <v>29</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>30</v>
@@ -1403,7 +1403,7 @@
         <v>36624</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H2" s="6">
         <v>1</v>
@@ -1447,7 +1447,7 @@
         <v>37810</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H3" s="9">
         <v>2</v>
@@ -1484,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:H42"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1534,10 +1534,10 @@
         <v>46</v>
       </c>
       <c r="J1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="20" t="s">
         <v>84</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>85</v>
       </c>
       <c r="L1" t="s">
         <v>44</v>
@@ -1582,7 +1582,7 @@
         <v>36910</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
@@ -1617,7 +1617,7 @@
         <v>36978</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
@@ -1652,7 +1652,7 @@
         <v>36484</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
@@ -1687,7 +1687,7 @@
         <v>36631</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
@@ -1724,7 +1724,7 @@
         <v>33073</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
@@ -1761,7 +1761,7 @@
         <v>38338</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
@@ -1798,7 +1798,7 @@
         <v>37166</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -1833,7 +1833,7 @@
         <v>37264</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
@@ -1868,7 +1868,7 @@
         <v>37200</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -1903,7 +1903,7 @@
         <v>36893</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
@@ -1935,7 +1935,7 @@
         <v>37880</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -1970,7 +1970,7 @@
         <v>37460</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
@@ -2002,7 +2002,7 @@
         <v>37504</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
@@ -2034,7 +2034,7 @@
         <v>38214</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T15" t="s">
         <v>53</v>
@@ -2069,7 +2069,7 @@
         <v>37691</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
@@ -2104,7 +2104,7 @@
         <v>34028</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2139,7 +2139,7 @@
         <v>38244</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
@@ -2168,13 +2168,13 @@
         <v>45260</v>
       </c>
       <c r="I19" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="J19" s="16">
         <v>32903</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
@@ -2203,13 +2203,13 @@
         <v>45260</v>
       </c>
       <c r="I20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J20" s="16">
         <v>37433</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
@@ -2241,7 +2241,7 @@
         <v>37936</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
@@ -2249,7 +2249,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C22" s="3">
         <v>11478</v>
@@ -2270,13 +2270,13 @@
         <v>45261</v>
       </c>
       <c r="I22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J22" s="16">
         <v>34393</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
@@ -2284,7 +2284,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="2">
         <v>10464</v>
@@ -2308,7 +2308,7 @@
         <v>35659</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
@@ -2316,7 +2316,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2">
         <v>10637</v>
@@ -2343,7 +2343,7 @@
         <v>37869</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M24" t="s">
         <v>53</v>
@@ -2354,7 +2354,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" s="2">
         <v>10443</v>
@@ -2378,7 +2378,7 @@
         <v>37670</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T25" t="s">
         <v>53</v>
@@ -2389,7 +2389,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" s="15">
         <v>11512</v>
@@ -2413,7 +2413,7 @@
         <v>37838</v>
       </c>
       <c r="K26" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
@@ -2421,7 +2421,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" s="3">
         <v>11124</v>
@@ -2445,7 +2445,7 @@
         <v>37040</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
@@ -2453,7 +2453,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28" s="3">
         <v>11600</v>
@@ -2477,7 +2477,7 @@
         <v>38142</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
@@ -2485,7 +2485,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29" s="3">
         <v>3061</v>
@@ -2509,7 +2509,7 @@
         <v>33365</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
@@ -2517,7 +2517,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" s="3">
         <v>11527</v>
@@ -2538,13 +2538,13 @@
         <v>45265</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J30" s="16">
         <v>37810</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
@@ -2552,7 +2552,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C31" s="3">
         <v>2317</v>
@@ -2576,7 +2576,7 @@
         <v>33146</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
@@ -2584,7 +2584,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C32" s="3">
         <v>8175</v>
@@ -2608,7 +2608,7 @@
         <v>32922</v>
       </c>
       <c r="K32" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -2616,7 +2616,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C33" s="3">
         <v>1697</v>
@@ -2640,7 +2640,7 @@
         <v>32661</v>
       </c>
       <c r="K33" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -2648,7 +2648,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C34" s="2">
         <v>9039</v>
@@ -2672,7 +2672,7 @@
         <v>35705</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -2680,7 +2680,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C35" s="3">
         <v>10010</v>
@@ -2704,7 +2704,7 @@
         <v>37475</v>
       </c>
       <c r="K35" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -2712,7 +2712,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C36" s="3">
         <v>10415</v>
@@ -2736,7 +2736,7 @@
         <v>37515</v>
       </c>
       <c r="K36" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -2744,7 +2744,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C37" s="3">
         <v>6729</v>
@@ -2768,7 +2768,7 @@
         <v>34059</v>
       </c>
       <c r="K37" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -2776,7 +2776,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C38" s="3">
         <v>11066</v>
@@ -2803,7 +2803,7 @@
         <v>37152</v>
       </c>
       <c r="K38" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -2811,7 +2811,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C39" s="2">
         <v>9245</v>
@@ -2832,13 +2832,13 @@
         <v>45273</v>
       </c>
       <c r="I39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J39" s="16">
         <v>36607</v>
       </c>
       <c r="K39" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -2846,7 +2846,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C40" s="2">
         <v>11067</v>
@@ -2870,7 +2870,7 @@
         <v>35101</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2878,7 +2878,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41" s="2">
         <v>8819</v>
@@ -2902,7 +2902,7 @@
         <v>35856</v>
       </c>
       <c r="K41" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -2910,7 +2910,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C42" s="15">
         <v>6210</v>
@@ -2934,7 +2934,7 @@
         <v>35934</v>
       </c>
       <c r="K42" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Textgrid Speak pts. 22-25, Praat files
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79240AD-F31B-449D-B651-DF9815DBC82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7925D578-5611-4A25-A800-A2DD4DA8DA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="105">
   <si>
     <t>Participant</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>Practice 1: She thought she had to name the colour. I corrected her and she got trials 5-12  right. Rather slow RTs. Speaks slowly.</t>
+  </si>
+  <si>
+    <t>Speaks very fast. Short durations.</t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1488,7 @@
   <dimension ref="A1:T49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2374,6 +2377,9 @@
       <c r="H25" s="14">
         <v>45261</v>
       </c>
+      <c r="I25" t="s">
+        <v>104</v>
+      </c>
       <c r="J25" s="16">
         <v>37670</v>
       </c>

</xml_diff>

<commit_message>
Textgrid Speak pts 26-27, Praat files
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7925D578-5611-4A25-A800-A2DD4DA8DA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92245D72-15E2-48DC-A40F-D06C7CE6D598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="106">
   <si>
     <t>Participant</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>Speaks very fast. Short durations.</t>
+  </si>
+  <si>
+    <t>Long durations</t>
   </si>
 </sst>
 </file>
@@ -1487,8 +1490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2479,6 +2482,9 @@
       <c r="H28" s="14">
         <v>45264</v>
       </c>
+      <c r="I28" t="s">
+        <v>105</v>
+      </c>
       <c r="J28" s="16">
         <v>38142</v>
       </c>

</xml_diff>

<commit_message>
renamed audio files pts 28-30
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92245D72-15E2-48DC-A40F-D06C7CE6D598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1C44C4-F1DE-4C65-B2A6-1DB86AD61506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1491,7 +1491,7 @@
   <dimension ref="A1:T49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Excel files pts 34-41
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1C44C4-F1DE-4C65-B2A6-1DB86AD61506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FE84BC-6187-4ED1-AA90-320B44EF9F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10188" yWindow="912" windowWidth="12852" windowHeight="12048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pilots" sheetId="3" r:id="rId1"/>

</xml_diff>

<commit_message>
Textgrid Speak pts 40-41, Praat output files
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FE84BC-6187-4ED1-AA90-320B44EF9F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE243D15-90ED-4943-8DAF-A11217949606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10188" yWindow="912" windowWidth="12852" windowHeight="12048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pilots" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="110">
   <si>
     <t>Participant</t>
   </si>
@@ -355,6 +355,18 @@
   </si>
   <si>
     <t>Long durations</t>
+  </si>
+  <si>
+    <t>Angelika Botero Montaña</t>
+  </si>
+  <si>
+    <t>Used words from South American Spanish in the familliarisation.</t>
+  </si>
+  <si>
+    <t>Alejandro Muñoz Pérez</t>
+  </si>
+  <si>
+    <t>In Practice2 I wrote his code ID as 430201 instead of 430102.</t>
   </si>
 </sst>
 </file>
@@ -1490,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2950,40 +2962,73 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43">
+      <c r="A43" s="2">
         <v>42</v>
       </c>
-      <c r="D43" s="1">
+      <c r="B43" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C43" s="3">
+        <v>10275</v>
+      </c>
+      <c r="D43" s="13">
         <v>420201</v>
       </c>
-      <c r="E43">
-        <v>2</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43" s="1" t="s">
+      <c r="E43" s="2">
+        <v>2</v>
+      </c>
+      <c r="F43" s="2">
+        <v>1</v>
+      </c>
+      <c r="G43" s="13" t="s">
         <v>48</v>
       </c>
+      <c r="H43" s="14">
+        <v>45307</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="J43" s="16">
+        <v>33061</v>
+      </c>
+      <c r="K43" s="19" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44">
+      <c r="A44" s="2">
         <v>43</v>
       </c>
-      <c r="D44" s="1">
+      <c r="B44" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="2">
+        <v>6835</v>
+      </c>
+      <c r="D44" s="13">
         <v>430102</v>
       </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-      <c r="F44">
-        <v>2</v>
-      </c>
-      <c r="G44" s="1" t="s">
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+      <c r="F44" s="2">
+        <v>2</v>
+      </c>
+      <c r="G44" s="13" t="s">
         <v>50</v>
       </c>
+      <c r="H44" s="14">
+        <v>45309</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J44" s="16">
+        <v>33718</v>
+      </c>
       <c r="K44" s="19" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -3073,11 +3118,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="D2 D5:D10 D4" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Textgrid Speak pts 28-29, Praat output files
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE243D15-90ED-4943-8DAF-A11217949606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A90072-F580-455D-97A8-614CB59888FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="112">
   <si>
     <t>Participant</t>
   </si>
@@ -367,6 +367,12 @@
   </si>
   <si>
     <t>In Practice2 I wrote his code ID as 430201 instead of 430102.</t>
+  </si>
+  <si>
+    <t>Patricia García Arenzana</t>
+  </si>
+  <si>
+    <t>Some RTs are close to 1200-1500ms</t>
   </si>
 </sst>
 </file>
@@ -1502,7 +1508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -2529,6 +2535,9 @@
       <c r="H29" s="14">
         <v>45264</v>
       </c>
+      <c r="I29" t="s">
+        <v>111</v>
+      </c>
       <c r="J29" s="16">
         <v>33365</v>
       </c>
@@ -2996,7 +3005,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -3032,20 +3041,35 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45">
+      <c r="A45" s="2">
         <v>44</v>
       </c>
-      <c r="D45" s="1">
+      <c r="B45" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="15">
+        <v>10964</v>
+      </c>
+      <c r="D45" s="13">
         <v>440202</v>
       </c>
-      <c r="E45">
-        <v>2</v>
-      </c>
-      <c r="F45">
-        <v>2</v>
-      </c>
-      <c r="G45" s="1" t="s">
+      <c r="E45" s="2">
+        <v>2</v>
+      </c>
+      <c r="F45" s="2">
+        <v>2</v>
+      </c>
+      <c r="G45" s="13" t="s">
         <v>22</v>
+      </c>
+      <c r="H45" s="14">
+        <v>45310</v>
+      </c>
+      <c r="J45" s="16">
+        <v>37441</v>
+      </c>
+      <c r="K45" s="19" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Textgrid Speak pt 35, Praat output files
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A90072-F580-455D-97A8-614CB59888FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86BDF53-99D0-4E94-BC45-AB3DE05DC952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="117">
   <si>
     <t>Participant</t>
   </si>
@@ -373,6 +373,21 @@
   </si>
   <si>
     <t>Some RTs are close to 1200-1500ms</t>
+  </si>
+  <si>
+    <t>RTs are relatively slow. Mostly between 1000-1400ms.</t>
+  </si>
+  <si>
+    <t>Relatively slow RTs -- between 1000 and 1500ms; some even close to 2sec. Long durations as well.</t>
+  </si>
+  <si>
+    <t>Leire Varela Aranguren</t>
+  </si>
+  <si>
+    <t>She can do the caja.</t>
+  </si>
+  <si>
+    <t>Lorena Muñoz Ruiz</t>
   </si>
 </sst>
 </file>
@@ -1508,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1519,7 +1534,7 @@
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" customWidth="1"/>
     <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.88671875" customWidth="1"/>
     <col min="10" max="10" width="13.44140625" customWidth="1"/>
     <col min="11" max="11" width="13.44140625" style="19" customWidth="1"/>
     <col min="12" max="13" width="10.5546875" customWidth="1"/>
@@ -2605,6 +2620,9 @@
       <c r="H31" s="14">
         <v>45265</v>
       </c>
+      <c r="I31" t="s">
+        <v>112</v>
+      </c>
       <c r="J31" s="16">
         <v>33146</v>
       </c>
@@ -2733,6 +2751,9 @@
       <c r="H35" s="4">
         <v>45272</v>
       </c>
+      <c r="I35" t="s">
+        <v>113</v>
+      </c>
       <c r="J35" s="16">
         <v>37475</v>
       </c>
@@ -3073,37 +3094,70 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46">
+      <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="D46" s="1">
+      <c r="B46" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" s="2">
+        <v>7789</v>
+      </c>
+      <c r="D46" s="13">
         <v>450103</v>
       </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46">
+      <c r="E46" s="2">
+        <v>1</v>
+      </c>
+      <c r="F46" s="2">
         <v>3</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="G46" s="13" t="s">
         <v>43</v>
       </c>
+      <c r="H46" s="14">
+        <v>45314</v>
+      </c>
+      <c r="I46" t="s">
+        <v>115</v>
+      </c>
+      <c r="J46" s="16">
+        <v>35886</v>
+      </c>
+      <c r="K46" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47">
+      <c r="A47" s="2">
         <v>46</v>
       </c>
-      <c r="D47" s="1">
+      <c r="B47" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" s="2">
+        <v>10942</v>
+      </c>
+      <c r="D47" s="13">
         <v>460203</v>
       </c>
-      <c r="E47">
-        <v>2</v>
-      </c>
-      <c r="F47">
+      <c r="E47" s="2">
+        <v>2</v>
+      </c>
+      <c r="F47" s="2">
         <v>3</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G47" s="13" t="s">
         <v>48</v>
+      </c>
+      <c r="H47" s="14">
+        <v>45315</v>
+      </c>
+      <c r="J47" s="16">
+        <v>38070</v>
+      </c>
+      <c r="K47" s="19" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
@@ -3122,6 +3176,7 @@
       <c r="G48" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="H48" s="16"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">

</xml_diff>

<commit_message>
Textgrid Speak pt. 37, Praat output files
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86BDF53-99D0-4E94-BC45-AB3DE05DC952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8C630E-64D3-4F55-85C7-122AD404478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="119">
   <si>
     <t>Participant</t>
   </si>
@@ -388,6 +388,12 @@
   </si>
   <si>
     <t>Lorena Muñoz Ruiz</t>
+  </si>
+  <si>
+    <t>490101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can do the caja! She has said and typed ´fresa´ instead of ´manzana´for all instances of the latter word. I checked the lists I use on PsychoPy and the output file from PsychoPy for that participant and the image used for the apple is that of an apple. </t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -535,6 +541,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1043,8 +1052,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}" name="Table1" displayName="Table1" ref="A1:O49" totalsRowShown="0">
-  <autoFilter ref="A1:O49" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}" name="Table1" displayName="Table1" ref="A1:O50" totalsRowShown="0">
+  <autoFilter ref="A1:O50" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{6A81B45A-EDC9-4FF5-8258-8648C067C16F}" name="Participant"/>
     <tableColumn id="5" xr3:uid="{23D0A20D-D062-4D9A-A44D-D77B8E1CBB39}" name="Name"/>
@@ -1521,10 +1530,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
-  <dimension ref="A1:T49"/>
+  <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:H47"/>
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2851,7 +2860,7 @@
         <v>45273</v>
       </c>
       <c r="I38" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="J38" s="16">
         <v>37152</v>
@@ -3176,9 +3185,11 @@
       <c r="G48" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H48" s="16"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H48" s="16">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3194,6 +3205,30 @@
       <c r="G49" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="H49" s="16">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H50" s="16">
+        <v>45317</v>
+      </c>
+      <c r="K50" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Textgrid Speak pts. 38-39, Praat output files
</commit_message>
<xml_diff>
--- a/documents/REPSWITCH_List.xlsx
+++ b/documents/REPSWITCH_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8C630E-64D3-4F55-85C7-122AD404478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D548848-BCB3-4CC3-8129-943CA0156624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4572" yWindow="972" windowWidth="12852" windowHeight="12048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pilots" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="124">
   <si>
     <t>Participant</t>
   </si>
@@ -394,6 +394,21 @@
   </si>
   <si>
     <t xml:space="preserve">Can do the caja! She has said and typed ´fresa´ instead of ´manzana´for all instances of the latter word. I checked the lists I use on PsychoPy and the output file from PsychoPy for that participant and the image used for the apple is that of an apple. </t>
+  </si>
+  <si>
+    <t>Naroa Borrajeros Elósegui</t>
+  </si>
+  <si>
+    <t>Thais Garcia Sevilla</t>
+  </si>
+  <si>
+    <t>Unai Roca</t>
+  </si>
+  <si>
+    <t>A bit sleepy. Can do the caja.</t>
+  </si>
+  <si>
+    <t>Has a cut on her right index. No issue in typing. Took off the bandage. Can do the caja.</t>
   </si>
 </sst>
 </file>
@@ -1052,8 +1067,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}" name="Table1" displayName="Table1" ref="A1:O50" totalsRowShown="0">
-  <autoFilter ref="A1:O50" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}" name="Table1" displayName="Table1" ref="A1:O51" totalsRowShown="0">
+  <autoFilter ref="A1:O51" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{6A81B45A-EDC9-4FF5-8258-8648C067C16F}" name="Participant"/>
     <tableColumn id="5" xr3:uid="{23D0A20D-D062-4D9A-A44D-D77B8E1CBB39}" name="Name"/>
@@ -1530,10 +1545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
-  <dimension ref="A1:T50"/>
+  <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3170,49 +3185,85 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48">
+      <c r="A48" s="2">
         <v>47</v>
       </c>
-      <c r="D48" s="1">
+      <c r="B48" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="3">
+        <v>6020</v>
+      </c>
+      <c r="D48" s="13">
         <v>470104</v>
       </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-      <c r="F48">
+      <c r="E48" s="2">
+        <v>1</v>
+      </c>
+      <c r="F48" s="2">
         <v>4</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="G48" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="H48" s="16">
+      <c r="H48" s="14">
         <v>45317</v>
       </c>
+      <c r="I48" t="s">
+        <v>122</v>
+      </c>
+      <c r="J48" s="16">
+        <v>36284</v>
+      </c>
+      <c r="K48" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="A49" s="2">
         <v>48</v>
       </c>
-      <c r="D49" s="1">
+      <c r="B49" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49" s="3">
+        <v>10038</v>
+      </c>
+      <c r="D49" s="13">
         <v>480204</v>
       </c>
-      <c r="E49">
-        <v>2</v>
-      </c>
-      <c r="F49">
+      <c r="E49" s="2">
+        <v>2</v>
+      </c>
+      <c r="F49" s="2">
         <v>4</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="G49" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H49" s="16">
+      <c r="H49" s="14">
         <v>45317</v>
+      </c>
+      <c r="I49" t="s">
+        <v>123</v>
+      </c>
+      <c r="J49" s="16">
+        <v>33386</v>
+      </c>
+      <c r="K49" s="19" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
+      <c r="B50" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" s="10">
+        <v>6477</v>
+      </c>
       <c r="D50" s="1" t="s">
         <v>117</v>
       </c>
@@ -3228,7 +3279,14 @@
       <c r="H50" s="16">
         <v>45317</v>
       </c>
-      <c r="K50" s="22"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="I51" t="s">
+        <v>53</v>
+      </c>
+      <c r="K51" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>